<commit_message>
Update Banco-BAC-14-Lenguaje en formatos.xlsx
</commit_message>
<xml_diff>
--- a/HT-1/Banco-BAC-14-Lenguaje en formatos.xlsx
+++ b/HT-1/Banco-BAC-14-Lenguaje en formatos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juan/Documents/Universidad/2022-20/arquiemp/repo/arquiemp/HT-1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC3CF97C-00E1-3B4D-9A1F-F2065947475A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12C26CEA-3CE7-884D-80A4-69622815F654}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-1700" windowWidth="38400" windowHeight="21100" xr2:uid="{6D2ADF59-F33A-44E3-88FB-8431094B32CC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="66">
   <si>
     <t>A Playbook for Business Architecture Construction</t>
   </si>
@@ -60,6 +60,9 @@
     <t>Cliente</t>
   </si>
   <si>
+    <t>PersonaNatural</t>
+  </si>
+  <si>
     <t>BAC-14 Lenguaje en formatos</t>
   </si>
   <si>
@@ -94,6 +97,141 @@
   </si>
   <si>
     <t>Cédula</t>
+  </si>
+  <si>
+    <t>BBVA</t>
+  </si>
+  <si>
+    <t>Itaú</t>
+  </si>
+  <si>
+    <t>Jorge Gutiérrez</t>
+  </si>
+  <si>
+    <t>Lucas Leal</t>
+  </si>
+  <si>
+    <t>Casa Toro</t>
+  </si>
+  <si>
+    <t>PersonaJurídica</t>
+  </si>
+  <si>
+    <t>Pichincha</t>
+  </si>
+  <si>
+    <t>Empanadas Típicas</t>
+  </si>
+  <si>
+    <t>Secretaría Distrital de Ambiente</t>
+  </si>
+  <si>
+    <t>Andrea Casablanca</t>
+  </si>
+  <si>
+    <t>Miguel Antonio Mejía</t>
+  </si>
+  <si>
+    <t>Colpatria</t>
+  </si>
+  <si>
+    <t>Marlon Andrés Casas</t>
+  </si>
+  <si>
+    <t>Universidad de los Andes</t>
+  </si>
+  <si>
+    <t>Acueducto de Bogotá</t>
+  </si>
+  <si>
+    <t>Bancolombia</t>
+  </si>
+  <si>
+    <t>Davivienda</t>
+  </si>
+  <si>
+    <t>Banco de occidente</t>
+  </si>
+  <si>
+    <t>Av Villas</t>
+  </si>
+  <si>
+    <t>Banco de Bogotá</t>
+  </si>
+  <si>
+    <t>830.004.993-8</t>
+  </si>
+  <si>
+    <t>900.612.118-1</t>
+  </si>
+  <si>
+    <t>899.999.061-9</t>
+  </si>
+  <si>
+    <t>899.999.094-1</t>
+  </si>
+  <si>
+    <t>860.007.386-1</t>
+  </si>
+  <si>
+    <t>Camila Palma</t>
+  </si>
+  <si>
+    <t>Rafael Marcos</t>
+  </si>
+  <si>
+    <t>Nicolás Naranjo</t>
+  </si>
+  <si>
+    <t>Luna Arce</t>
+  </si>
+  <si>
+    <t>Pablo Iñiguez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ildefonso Gil </t>
+  </si>
+  <si>
+    <t>Edgardo Cabezas</t>
+  </si>
+  <si>
+    <t>Sancho Angulo</t>
+  </si>
+  <si>
+    <t>Evelia Jordán</t>
+  </si>
+  <si>
+    <t>Eric Rubio</t>
+  </si>
+  <si>
+    <t>Nacho Coello</t>
+  </si>
+  <si>
+    <t>Jenaro Rosell</t>
+  </si>
+  <si>
+    <t>Paula Sans</t>
+  </si>
+  <si>
+    <t>Cajero</t>
+  </si>
+  <si>
+    <t>Agente de ventas</t>
+  </si>
+  <si>
+    <t>Contador</t>
+  </si>
+  <si>
+    <t>Administrador</t>
+  </si>
+  <si>
+    <t>Jefe de marketing</t>
+  </si>
+  <si>
+    <t>Atencion al cliente</t>
+  </si>
+  <si>
+    <t>Jefe de TI</t>
   </si>
 </sst>
 </file>
@@ -135,7 +273,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -195,14 +333,81 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -214,9 +419,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -230,6 +432,45 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -547,380 +788,581 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ABDEE2F-9DA5-4F4F-A9BF-B9BEA22ACD0E}">
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" customWidth="1"/>
+    <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" customWidth="1"/>
     <col min="3" max="3" width="15.5" customWidth="1"/>
+    <col min="4" max="4" width="27.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
     </row>
     <row r="2" spans="1:13" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+    </row>
+    <row r="3" spans="1:13" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
     </row>
     <row r="4" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
     </row>
     <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="G5" s="10" t="s">
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="G5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="11"/>
-      <c r="I5" s="10" t="s">
+      <c r="H5" s="9"/>
+      <c r="I5" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="J5" s="12"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="10" t="s">
+      <c r="J5" s="10"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="M5" s="11"/>
+      <c r="M5" s="9"/>
     </row>
     <row r="6" spans="1:13" ht="15" x14ac:dyDescent="0.15">
-      <c r="A6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="6" t="s">
+      <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="5" t="s">
+      <c r="C6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="D6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="E6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="H6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="15" x14ac:dyDescent="0.15">
+      <c r="A7" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="19">
+        <v>1000563143</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="6">
+        <v>3102318734</v>
+      </c>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+    </row>
+    <row r="8" spans="1:13" ht="15" x14ac:dyDescent="0.15">
+      <c r="A8" s="14"/>
+      <c r="B8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="19">
+        <v>1074932089</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="6">
+        <v>3210753951</v>
+      </c>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+    </row>
+    <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="15"/>
+      <c r="B9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="6">
+        <v>3208943567</v>
+      </c>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+    </row>
+    <row r="10" spans="1:13" ht="15" x14ac:dyDescent="0.15">
+      <c r="A10" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="6">
+        <v>3150291735</v>
+      </c>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+    </row>
+    <row r="11" spans="1:13" ht="15" x14ac:dyDescent="0.15">
+      <c r="A11" s="14"/>
+      <c r="B11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="6">
+        <v>3142138410</v>
+      </c>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+    </row>
+    <row r="12" spans="1:13" ht="15" x14ac:dyDescent="0.15">
+      <c r="A12" s="14"/>
+      <c r="B12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="19">
+        <v>1012906107</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="6">
+        <v>3132023149</v>
+      </c>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+    </row>
+    <row r="13" spans="1:13" ht="15" x14ac:dyDescent="0.15">
+      <c r="A13" s="15"/>
+      <c r="B13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="19">
+        <v>1062123530</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="6">
+        <v>3103213842</v>
+      </c>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+    </row>
+    <row r="14" spans="1:13" ht="15" x14ac:dyDescent="0.15">
+      <c r="A14" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="19">
+        <v>1001321342</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="6">
+        <v>3192031942</v>
+      </c>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+    </row>
+    <row r="15" spans="1:13" ht="15" x14ac:dyDescent="0.15">
+      <c r="A15" s="17"/>
+      <c r="B15" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="6">
+        <v>3142137283</v>
+      </c>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+    </row>
+    <row r="16" spans="1:13" ht="15" x14ac:dyDescent="0.15">
+      <c r="A16" s="18"/>
+      <c r="B16" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" s="6">
+        <v>3172183921</v>
+      </c>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+    </row>
+    <row r="19" spans="1:7" ht="15" x14ac:dyDescent="0.15">
+      <c r="A19" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" s="10"/>
+      <c r="G19" s="9"/>
+    </row>
+    <row r="20" spans="1:7" ht="15" x14ac:dyDescent="0.15">
+      <c r="A20" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J6" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K6" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="L6" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="M6" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A7" s="7"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A8" s="7"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A9" s="7"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A10" s="7"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A11" s="7"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A12" s="7"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
-      <c r="M13" s="8"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8"/>
-      <c r="M14" s="8"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="8"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
-      <c r="M16" s="8"/>
-    </row>
-    <row r="19" spans="1:7" ht="15" x14ac:dyDescent="0.15">
-      <c r="A19" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="F19" s="12"/>
-      <c r="G19" s="11"/>
-    </row>
-    <row r="20" spans="1:7" ht="15" x14ac:dyDescent="0.15">
-      <c r="A20" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E20" s="6" t="s">
+      <c r="B20" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F20" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G20" s="6" t="s">
+      <c r="D20" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="5" t="s">
         <v>19</v>
       </c>
+      <c r="F20" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
+      <c r="A21" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="6"/>
+      <c r="D21" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G21" s="23">
+        <v>1003794201</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
+      <c r="A22" s="21"/>
+      <c r="B22" s="6"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="G22" s="23">
+        <v>1002102314</v>
+      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
+      <c r="A23" s="21"/>
+      <c r="B23" s="6"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="G23" s="23">
+        <v>1002112425</v>
+      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A24" s="8"/>
-      <c r="B24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
+      <c r="A24" s="21"/>
+      <c r="B24" s="6"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="G24" s="23">
+        <v>1000495015</v>
+      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A25" s="8"/>
-      <c r="B25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
+      <c r="A25" s="22"/>
+      <c r="B25" s="6"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="G25" s="23">
+        <v>1100592356</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
+      <c r="A26" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="6"/>
+      <c r="D26" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="G26" s="23">
+        <v>1043242892</v>
+      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A27" s="8"/>
-      <c r="B27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
+      <c r="A27" s="14"/>
+      <c r="B27" s="6"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G27" s="23">
+        <v>1000042718</v>
+      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A28" s="8"/>
-      <c r="B28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
+      <c r="A28" s="14"/>
+      <c r="B28" s="6"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="G28" s="23">
+        <v>1047506124</v>
+      </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A29" s="8"/>
-      <c r="B29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
+      <c r="A29" s="15"/>
+      <c r="B29" s="6"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="G29" s="23">
+        <v>1001232031</v>
+      </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A30" s="8"/>
-      <c r="B30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
+      <c r="A30" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30" s="6"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G30" s="23">
+        <v>1100392576</v>
+      </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A31" s="8"/>
-      <c r="B31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
+      <c r="A31" s="14"/>
+      <c r="B31" s="6"/>
+      <c r="D31" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="G31" s="23">
+        <v>1213134523</v>
+      </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A32" s="8"/>
-      <c r="B32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
+      <c r="A32" s="14"/>
+      <c r="B32" s="6"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="G32" s="23">
+        <v>1200313498</v>
+      </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A33" s="8"/>
-      <c r="B33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
+      <c r="A33" s="15"/>
+      <c r="B33" s="6"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G33" s="23">
+        <v>1000232569</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="17">
+    <mergeCell ref="A21:A25"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="D21:D25"/>
+    <mergeCell ref="D26:D30"/>
+    <mergeCell ref="D31:D33"/>
     <mergeCell ref="E19:G19"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="A14:A16"/>
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="I5:K5"/>

</xml_diff>